<commit_message>
Refactor song evaluation process to use user input text instead of file path, update leaderboard handling, and add new API endpoints for leaderboard generation and backend health check. Also, enhance error handling and improve code structure for better readability.
</commit_message>
<xml_diff>
--- a/backends/data/Prompt Engineering Songs.xlsx
+++ b/backends/data/Prompt Engineering Songs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28627"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lyla/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://elonuniversity-my.sharepoint.com/personal/makben_elon_edu/Documents/AI Integration/2024/Projects/2025-DataNexus/DataNexusAI/backends/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{FFDCBE26-57FD-3040-9AEF-B73506820D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FEA118FD-8033-4C75-9895-80ACE4FDE87F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3155,7 +3155,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3531,15 +3531,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3554,7 +3554,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" ht="176.1">
+    <row r="2" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -3569,7 +3569,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="207.95">
+    <row r="3" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -3584,7 +3584,7 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="207.95">
+    <row r="4" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -3599,7 +3599,7 @@
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="159.94999999999999">
+    <row r="5" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -3614,7 +3614,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" ht="224.1">
+    <row r="6" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -3629,7 +3629,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="272.10000000000002">
+    <row r="7" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -3644,7 +3644,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="159.94999999999999">
+    <row r="8" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
@@ -3659,7 +3659,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" ht="224.1">
+    <row r="9" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -3674,7 +3674,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="192">
+    <row r="10" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>29</v>
       </c>
@@ -3689,7 +3689,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="207.95">
+    <row r="11" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -3704,7 +3704,7 @@
       </c>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="176.1">
+    <row r="12" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>34</v>
       </c>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="255.95">
+    <row r="13" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>37</v>
       </c>
@@ -3734,7 +3734,7 @@
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="192">
+    <row r="14" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -3749,7 +3749,7 @@
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="207.95">
+    <row r="15" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -3764,7 +3764,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="240">
+    <row r="16" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -3779,7 +3779,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="192">
+    <row r="17" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>49</v>
       </c>
@@ -3794,7 +3794,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="192">
+    <row r="18" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>52</v>
       </c>
@@ -3809,7 +3809,7 @@
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" ht="207.95">
+    <row r="19" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>54</v>
       </c>
@@ -3824,7 +3824,7 @@
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" ht="176.1">
+    <row r="20" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>57</v>
       </c>
@@ -3839,7 +3839,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" ht="159.94999999999999">
+    <row r="21" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>60</v>
       </c>
@@ -3854,7 +3854,7 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" ht="207.95">
+    <row r="22" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
@@ -3869,7 +3869,7 @@
       </c>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" ht="192">
+    <row r="23" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>66</v>
       </c>
@@ -3884,7 +3884,7 @@
       </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" ht="224.1">
+    <row r="24" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>69</v>
       </c>
@@ -3899,7 +3899,7 @@
       </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" ht="224.1">
+    <row r="25" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>72</v>
       </c>
@@ -3914,7 +3914,7 @@
       </c>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" ht="176.1">
+    <row r="26" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>75</v>
       </c>
@@ -3929,7 +3929,7 @@
       </c>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" ht="255.95">
+    <row r="27" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>78</v>
       </c>
@@ -3944,7 +3944,7 @@
       </c>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="1:5" ht="176.1">
+    <row r="28" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>80</v>
       </c>
@@ -3959,7 +3959,7 @@
       </c>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" ht="224.1">
+    <row r="29" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>83</v>
       </c>
@@ -3974,7 +3974,7 @@
       </c>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" ht="192">
+    <row r="30" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>86</v>
       </c>
@@ -3989,7 +3989,7 @@
       </c>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" ht="192">
+    <row r="31" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>88</v>
       </c>
@@ -4004,7 +4004,7 @@
       </c>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" ht="207.95">
+    <row r="32" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>90</v>
       </c>
@@ -4019,7 +4019,7 @@
       </c>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" ht="192">
+    <row r="33" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>92</v>
       </c>
@@ -4034,7 +4034,7 @@
       </c>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" ht="224.1">
+    <row r="34" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>95</v>
       </c>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" ht="224.1">
+    <row r="35" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>97</v>
       </c>
@@ -4064,7 +4064,7 @@
       </c>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" ht="255.95">
+    <row r="36" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>99</v>
       </c>
@@ -4079,7 +4079,7 @@
       </c>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" ht="350.1">
+    <row r="37" spans="1:5" ht="319" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>101</v>
       </c>
@@ -4094,7 +4094,7 @@
       </c>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" ht="192">
+    <row r="38" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>103</v>
       </c>
@@ -4109,7 +4109,7 @@
       </c>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5" ht="224.1">
+    <row r="39" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>106</v>
       </c>
@@ -4124,7 +4124,7 @@
       </c>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5" ht="255.95">
+    <row r="40" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>109</v>
       </c>
@@ -4139,7 +4139,7 @@
       </c>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5" ht="255.95">
+    <row r="41" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>112</v>
       </c>
@@ -4154,7 +4154,7 @@
       </c>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5" ht="207.95">
+    <row r="42" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>114</v>
       </c>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5" ht="192">
+    <row r="43" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>118</v>
       </c>
@@ -4184,7 +4184,7 @@
       </c>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5" ht="224.1">
+    <row r="44" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>121</v>
       </c>
@@ -4199,7 +4199,7 @@
       </c>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5" ht="303.95">
+    <row r="45" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>124</v>
       </c>
@@ -4214,7 +4214,7 @@
       </c>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5" ht="240">
+    <row r="46" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>127</v>
       </c>
@@ -4229,7 +4229,7 @@
       </c>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="1:5" ht="303.95">
+    <row r="47" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>130</v>
       </c>
@@ -4244,7 +4244,7 @@
       </c>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:5" ht="207.95">
+    <row r="48" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>132</v>
       </c>
@@ -4259,7 +4259,7 @@
       </c>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="1:5" ht="320.10000000000002">
+    <row r="49" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>134</v>
       </c>
@@ -4274,7 +4274,7 @@
       </c>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="1:5" ht="255.95">
+    <row r="50" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>137</v>
       </c>
@@ -4289,7 +4289,7 @@
       </c>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="1:5" ht="288">
+    <row r="51" spans="1:5" ht="290" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>140</v>
       </c>
@@ -4304,7 +4304,7 @@
       </c>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="1:5" ht="224.1">
+    <row r="52" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>143</v>
       </c>
@@ -4319,7 +4319,7 @@
       </c>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="1:5" ht="192">
+    <row r="53" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>145</v>
       </c>
@@ -4334,7 +4334,7 @@
       </c>
       <c r="E53" s="1"/>
     </row>
-    <row r="54" spans="1:5" ht="224.1">
+    <row r="54" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>148</v>
       </c>
@@ -4349,7 +4349,7 @@
       </c>
       <c r="E54" s="1"/>
     </row>
-    <row r="55" spans="1:5" ht="224.1">
+    <row r="55" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>151</v>
       </c>
@@ -4364,7 +4364,7 @@
       </c>
       <c r="E55" s="1"/>
     </row>
-    <row r="56" spans="1:5" ht="192">
+    <row r="56" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>153</v>
       </c>
@@ -4379,7 +4379,7 @@
       </c>
       <c r="E56" s="1"/>
     </row>
-    <row r="57" spans="1:5" ht="255.95">
+    <row r="57" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>156</v>
       </c>
@@ -4394,7 +4394,7 @@
       </c>
       <c r="E57" s="1"/>
     </row>
-    <row r="58" spans="1:5" ht="207.95">
+    <row r="58" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>159</v>
       </c>
@@ -4409,7 +4409,7 @@
       </c>
       <c r="E58" s="1"/>
     </row>
-    <row r="59" spans="1:5" ht="272.10000000000002">
+    <row r="59" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>162</v>
       </c>
@@ -4424,7 +4424,7 @@
       </c>
       <c r="E59" s="1"/>
     </row>
-    <row r="60" spans="1:5" ht="224.1">
+    <row r="60" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>165</v>
       </c>
@@ -4439,7 +4439,7 @@
       </c>
       <c r="E60" s="1"/>
     </row>
-    <row r="61" spans="1:5" ht="240">
+    <row r="61" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>167</v>
       </c>
@@ -4454,7 +4454,7 @@
       </c>
       <c r="E61" s="1"/>
     </row>
-    <row r="62" spans="1:5" ht="207.95">
+    <row r="62" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>170</v>
       </c>
@@ -4469,7 +4469,7 @@
       </c>
       <c r="E62" s="1"/>
     </row>
-    <row r="63" spans="1:5" ht="255.95">
+    <row r="63" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>173</v>
       </c>
@@ -4484,7 +4484,7 @@
       </c>
       <c r="E63" s="1"/>
     </row>
-    <row r="64" spans="1:5" ht="207.95">
+    <row r="64" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>176</v>
       </c>
@@ -4499,7 +4499,7 @@
       </c>
       <c r="E64" s="1"/>
     </row>
-    <row r="65" spans="1:5" ht="192">
+    <row r="65" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>179</v>
       </c>
@@ -4514,7 +4514,7 @@
       </c>
       <c r="E65" s="1"/>
     </row>
-    <row r="66" spans="1:5" ht="272.10000000000002">
+    <row r="66" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>182</v>
       </c>
@@ -4529,7 +4529,7 @@
       </c>
       <c r="E66" s="1"/>
     </row>
-    <row r="67" spans="1:5" ht="144">
+    <row r="67" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>185</v>
       </c>
@@ -4544,7 +4544,7 @@
       </c>
       <c r="E67" s="1"/>
     </row>
-    <row r="68" spans="1:5" ht="224.1">
+    <row r="68" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>188</v>
       </c>
@@ -4559,7 +4559,7 @@
       </c>
       <c r="E68" s="1"/>
     </row>
-    <row r="69" spans="1:5" ht="159.94999999999999">
+    <row r="69" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>191</v>
       </c>
@@ -4574,7 +4574,7 @@
       </c>
       <c r="E69" s="1"/>
     </row>
-    <row r="70" spans="1:5" ht="207.95">
+    <row r="70" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>194</v>
       </c>
@@ -4589,7 +4589,7 @@
       </c>
       <c r="E70" s="1"/>
     </row>
-    <row r="71" spans="1:5" ht="255.95">
+    <row r="71" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>197</v>
       </c>
@@ -4604,7 +4604,7 @@
       </c>
       <c r="E71" s="1"/>
     </row>
-    <row r="72" spans="1:5" ht="176.1">
+    <row r="72" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>199</v>
       </c>
@@ -4619,7 +4619,7 @@
       </c>
       <c r="E72" s="1"/>
     </row>
-    <row r="73" spans="1:5" ht="288">
+    <row r="73" spans="1:5" ht="290" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>202</v>
       </c>
@@ -4634,7 +4634,7 @@
       </c>
       <c r="E73" s="1"/>
     </row>
-    <row r="74" spans="1:5" ht="255.95">
+    <row r="74" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>205</v>
       </c>
@@ -4649,7 +4649,7 @@
       </c>
       <c r="E74" s="1"/>
     </row>
-    <row r="75" spans="1:5" ht="224.1">
+    <row r="75" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>208</v>
       </c>
@@ -4664,7 +4664,7 @@
       </c>
       <c r="E75" s="1"/>
     </row>
-    <row r="76" spans="1:5" ht="240">
+    <row r="76" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>211</v>
       </c>
@@ -4679,7 +4679,7 @@
       </c>
       <c r="E76" s="1"/>
     </row>
-    <row r="77" spans="1:5" ht="255.95">
+    <row r="77" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>214</v>
       </c>
@@ -4694,7 +4694,7 @@
       </c>
       <c r="E77" s="1"/>
     </row>
-    <row r="78" spans="1:5" ht="303.95">
+    <row r="78" spans="1:5" ht="290" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>217</v>
       </c>
@@ -4709,7 +4709,7 @@
       </c>
       <c r="E78" s="1"/>
     </row>
-    <row r="79" spans="1:5" ht="224.1">
+    <row r="79" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>220</v>
       </c>
@@ -4724,7 +4724,7 @@
       </c>
       <c r="E79" s="1"/>
     </row>
-    <row r="80" spans="1:5" ht="192">
+    <row r="80" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>223</v>
       </c>
@@ -4739,7 +4739,7 @@
       </c>
       <c r="E80" s="1"/>
     </row>
-    <row r="81" spans="1:5" ht="207.95">
+    <row r="81" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>114</v>
       </c>
@@ -4754,7 +4754,7 @@
       </c>
       <c r="E81" s="1"/>
     </row>
-    <row r="82" spans="1:5" ht="255.95">
+    <row r="82" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>226</v>
       </c>
@@ -4769,7 +4769,7 @@
       </c>
       <c r="E82" s="1"/>
     </row>
-    <row r="83" spans="1:5" ht="288">
+    <row r="83" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>230</v>
       </c>
@@ -4784,7 +4784,7 @@
       </c>
       <c r="E83" s="1"/>
     </row>
-    <row r="84" spans="1:5" ht="176.1">
+    <row r="84" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>233</v>
       </c>
@@ -4799,7 +4799,7 @@
       </c>
       <c r="E84" s="1"/>
     </row>
-    <row r="85" spans="1:5" ht="207.95">
+    <row r="85" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>236</v>
       </c>
@@ -4814,7 +4814,7 @@
       </c>
       <c r="E85" s="1"/>
     </row>
-    <row r="86" spans="1:5" ht="192">
+    <row r="86" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>239</v>
       </c>
@@ -4829,7 +4829,7 @@
       </c>
       <c r="E86" s="1"/>
     </row>
-    <row r="87" spans="1:5" ht="224.1">
+    <row r="87" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>241</v>
       </c>
@@ -4844,7 +4844,7 @@
       </c>
       <c r="E87" s="1"/>
     </row>
-    <row r="88" spans="1:5" ht="207.95">
+    <row r="88" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>244</v>
       </c>
@@ -4859,7 +4859,7 @@
       </c>
       <c r="E88" s="1"/>
     </row>
-    <row r="89" spans="1:5" ht="159.94999999999999">
+    <row r="89" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>246</v>
       </c>
@@ -4874,7 +4874,7 @@
       </c>
       <c r="E89" s="1"/>
     </row>
-    <row r="90" spans="1:5" ht="255.95">
+    <row r="90" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>248</v>
       </c>
@@ -4889,7 +4889,7 @@
       </c>
       <c r="E90" s="1"/>
     </row>
-    <row r="91" spans="1:5" ht="240">
+    <row r="91" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>251</v>
       </c>
@@ -4904,7 +4904,7 @@
       </c>
       <c r="E91" s="1"/>
     </row>
-    <row r="92" spans="1:5" ht="207.95">
+    <row r="92" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>254</v>
       </c>
@@ -4919,7 +4919,7 @@
       </c>
       <c r="E92" s="1"/>
     </row>
-    <row r="93" spans="1:5" ht="255.95">
+    <row r="93" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>257</v>
       </c>
@@ -4934,7 +4934,7 @@
       </c>
       <c r="E93" s="1"/>
     </row>
-    <row r="94" spans="1:5" ht="207.95">
+    <row r="94" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A94" s="1" t="s">
         <v>260</v>
       </c>
@@ -4949,7 +4949,7 @@
       </c>
       <c r="E94" s="1"/>
     </row>
-    <row r="95" spans="1:5" ht="192">
+    <row r="95" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A95" s="1" t="s">
         <v>263</v>
       </c>
@@ -4964,7 +4964,7 @@
       </c>
       <c r="E95" s="1"/>
     </row>
-    <row r="96" spans="1:5" ht="240">
+    <row r="96" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A96" s="1" t="s">
         <v>266</v>
       </c>
@@ -4979,7 +4979,7 @@
       </c>
       <c r="E96" s="1"/>
     </row>
-    <row r="97" spans="1:5" ht="224.1">
+    <row r="97" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A97" s="1" t="s">
         <v>269</v>
       </c>
@@ -4994,7 +4994,7 @@
       </c>
       <c r="E97" s="1"/>
     </row>
-    <row r="98" spans="1:5" ht="224.1">
+    <row r="98" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A98" s="1" t="s">
         <v>271</v>
       </c>
@@ -5009,7 +5009,7 @@
       </c>
       <c r="E98" s="1"/>
     </row>
-    <row r="99" spans="1:5" ht="272.10000000000002">
+    <row r="99" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>274</v>
       </c>
@@ -5024,7 +5024,7 @@
       </c>
       <c r="E99" s="1"/>
     </row>
-    <row r="100" spans="1:5" ht="255.95">
+    <row r="100" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A100" s="1" t="s">
         <v>276</v>
       </c>
@@ -5039,7 +5039,7 @@
       </c>
       <c r="E100" s="1"/>
     </row>
-    <row r="101" spans="1:5" ht="224.1">
+    <row r="101" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A101" s="1" t="s">
         <v>279</v>
       </c>
@@ -5054,7 +5054,7 @@
       </c>
       <c r="E101" s="1"/>
     </row>
-    <row r="102" spans="1:5" ht="224.1">
+    <row r="102" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>282</v>
       </c>
@@ -5069,7 +5069,7 @@
       </c>
       <c r="E102" s="1"/>
     </row>
-    <row r="103" spans="1:5" ht="224.1">
+    <row r="103" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A103" s="1" t="s">
         <v>284</v>
       </c>
@@ -5084,7 +5084,7 @@
       </c>
       <c r="E103" s="1"/>
     </row>
-    <row r="104" spans="1:5" ht="288">
+    <row r="104" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>287</v>
       </c>
@@ -5099,7 +5099,7 @@
       </c>
       <c r="E104" s="1"/>
     </row>
-    <row r="105" spans="1:5" ht="207.95">
+    <row r="105" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A105" s="1" t="s">
         <v>290</v>
       </c>
@@ -5114,7 +5114,7 @@
       </c>
       <c r="E105" s="1"/>
     </row>
-    <row r="106" spans="1:5" ht="272.10000000000002">
+    <row r="106" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>293</v>
       </c>
@@ -5129,7 +5129,7 @@
       </c>
       <c r="E106" s="1"/>
     </row>
-    <row r="107" spans="1:5" ht="207.95">
+    <row r="107" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A107" s="1" t="s">
         <v>295</v>
       </c>
@@ -5144,7 +5144,7 @@
       </c>
       <c r="E107" s="1"/>
     </row>
-    <row r="108" spans="1:5" ht="224.1">
+    <row r="108" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A108" s="1" t="s">
         <v>298</v>
       </c>
@@ -5159,7 +5159,7 @@
       </c>
       <c r="E108" s="1"/>
     </row>
-    <row r="109" spans="1:5" ht="255.95">
+    <row r="109" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A109" s="1" t="s">
         <v>301</v>
       </c>
@@ -5174,7 +5174,7 @@
       </c>
       <c r="E109" s="1"/>
     </row>
-    <row r="110" spans="1:5" ht="176.1">
+    <row r="110" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A110" s="1" t="s">
         <v>303</v>
       </c>
@@ -5189,7 +5189,7 @@
       </c>
       <c r="E110" s="1"/>
     </row>
-    <row r="111" spans="1:5" ht="240">
+    <row r="111" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A111" s="1" t="s">
         <v>306</v>
       </c>
@@ -5204,7 +5204,7 @@
       </c>
       <c r="E111" s="1"/>
     </row>
-    <row r="112" spans="1:5" ht="192">
+    <row r="112" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A112" s="1" t="s">
         <v>308</v>
       </c>
@@ -5219,7 +5219,7 @@
       </c>
       <c r="E112" s="1"/>
     </row>
-    <row r="113" spans="1:5" ht="159.94999999999999">
+    <row r="113" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A113" s="1" t="s">
         <v>311</v>
       </c>
@@ -5234,7 +5234,7 @@
       </c>
       <c r="E113" s="1"/>
     </row>
-    <row r="114" spans="1:5" ht="224.1">
+    <row r="114" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A114" s="1" t="s">
         <v>314</v>
       </c>
@@ -5249,7 +5249,7 @@
       </c>
       <c r="E114" s="1"/>
     </row>
-    <row r="115" spans="1:5" ht="288">
+    <row r="115" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A115" s="1" t="s">
         <v>317</v>
       </c>
@@ -5264,7 +5264,7 @@
       </c>
       <c r="E115" s="1"/>
     </row>
-    <row r="116" spans="1:5" ht="240">
+    <row r="116" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A116" s="1" t="s">
         <v>320</v>
       </c>
@@ -5279,7 +5279,7 @@
       </c>
       <c r="E116" s="1"/>
     </row>
-    <row r="117" spans="1:5" ht="240">
+    <row r="117" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A117" s="1" t="s">
         <v>323</v>
       </c>
@@ -5294,7 +5294,7 @@
       </c>
       <c r="E117" s="1"/>
     </row>
-    <row r="118" spans="1:5" ht="192">
+    <row r="118" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>326</v>
       </c>
@@ -5309,7 +5309,7 @@
       </c>
       <c r="E118" s="1"/>
     </row>
-    <row r="119" spans="1:5" ht="207.95">
+    <row r="119" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A119" s="1" t="s">
         <v>329</v>
       </c>
@@ -5324,7 +5324,7 @@
       </c>
       <c r="E119" s="1"/>
     </row>
-    <row r="120" spans="1:5" ht="176.1">
+    <row r="120" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A120" s="1" t="s">
         <v>332</v>
       </c>
@@ -5339,7 +5339,7 @@
       </c>
       <c r="E120" s="1"/>
     </row>
-    <row r="121" spans="1:5" ht="224.1">
+    <row r="121" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A121" s="1" t="s">
         <v>226</v>
       </c>
@@ -5354,7 +5354,7 @@
       </c>
       <c r="E121" s="1"/>
     </row>
-    <row r="122" spans="1:5" ht="207.95">
+    <row r="122" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A122" s="1" t="s">
         <v>336</v>
       </c>
@@ -5369,7 +5369,7 @@
       </c>
       <c r="E122" s="1"/>
     </row>
-    <row r="123" spans="1:5" ht="192">
+    <row r="123" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A123" s="1" t="s">
         <v>340</v>
       </c>
@@ -5384,7 +5384,7 @@
       </c>
       <c r="E123" s="1"/>
     </row>
-    <row r="124" spans="1:5" ht="207.95">
+    <row r="124" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A124" s="1" t="s">
         <v>343</v>
       </c>
@@ -5399,7 +5399,7 @@
       </c>
       <c r="E124" s="1"/>
     </row>
-    <row r="125" spans="1:5" ht="192">
+    <row r="125" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A125" s="1" t="s">
         <v>346</v>
       </c>
@@ -5414,7 +5414,7 @@
       </c>
       <c r="E125" s="1"/>
     </row>
-    <row r="126" spans="1:5" ht="240">
+    <row r="126" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
         <v>348</v>
       </c>
@@ -5429,7 +5429,7 @@
       </c>
       <c r="E126" s="1"/>
     </row>
-    <row r="127" spans="1:5" ht="272.10000000000002">
+    <row r="127" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
         <v>351</v>
       </c>
@@ -5444,7 +5444,7 @@
       </c>
       <c r="E127" s="1"/>
     </row>
-    <row r="128" spans="1:5" ht="207.95">
+    <row r="128" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A128" s="1" t="s">
         <v>354</v>
       </c>
@@ -5459,7 +5459,7 @@
       </c>
       <c r="E128" s="1"/>
     </row>
-    <row r="129" spans="1:5" ht="192">
+    <row r="129" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A129" s="1" t="s">
         <v>356</v>
       </c>
@@ -5474,7 +5474,7 @@
       </c>
       <c r="E129" s="1"/>
     </row>
-    <row r="130" spans="1:5" ht="176.1">
+    <row r="130" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A130" s="1" t="s">
         <v>359</v>
       </c>
@@ -5489,7 +5489,7 @@
       </c>
       <c r="E130" s="1"/>
     </row>
-    <row r="131" spans="1:5" ht="255.95">
+    <row r="131" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A131" s="1" t="s">
         <v>362</v>
       </c>
@@ -5504,7 +5504,7 @@
       </c>
       <c r="E131" s="1"/>
     </row>
-    <row r="132" spans="1:5" ht="224.1">
+    <row r="132" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A132" s="1" t="s">
         <v>364</v>
       </c>
@@ -5519,7 +5519,7 @@
       </c>
       <c r="E132" s="1"/>
     </row>
-    <row r="133" spans="1:5" ht="176.1">
+    <row r="133" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A133" s="1" t="s">
         <v>367</v>
       </c>
@@ -5534,7 +5534,7 @@
       </c>
       <c r="E133" s="1"/>
     </row>
-    <row r="134" spans="1:5" ht="255.95">
+    <row r="134" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
         <v>370</v>
       </c>
@@ -5549,7 +5549,7 @@
       </c>
       <c r="E134" s="1"/>
     </row>
-    <row r="135" spans="1:5" ht="207.95">
+    <row r="135" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
         <v>373</v>
       </c>
@@ -5564,7 +5564,7 @@
       </c>
       <c r="E135" s="1"/>
     </row>
-    <row r="136" spans="1:5" ht="192">
+    <row r="136" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A136" s="1" t="s">
         <v>375</v>
       </c>
@@ -5579,7 +5579,7 @@
       </c>
       <c r="E136" s="1"/>
     </row>
-    <row r="137" spans="1:5" ht="207.95">
+    <row r="137" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A137" s="1" t="s">
         <v>378</v>
       </c>
@@ -5594,7 +5594,7 @@
       </c>
       <c r="E137" s="1"/>
     </row>
-    <row r="138" spans="1:5" ht="240">
+    <row r="138" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A138" s="1" t="s">
         <v>380</v>
       </c>
@@ -5609,7 +5609,7 @@
       </c>
       <c r="E138" s="1"/>
     </row>
-    <row r="139" spans="1:5" ht="255.95">
+    <row r="139" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A139" s="1" t="s">
         <v>223</v>
       </c>
@@ -5624,7 +5624,7 @@
       </c>
       <c r="E139" s="1"/>
     </row>
-    <row r="140" spans="1:5" ht="176.1">
+    <row r="140" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A140" s="1" t="s">
         <v>384</v>
       </c>
@@ -5639,7 +5639,7 @@
       </c>
       <c r="E140" s="1"/>
     </row>
-    <row r="141" spans="1:5" ht="176.1">
+    <row r="141" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A141" s="1" t="s">
         <v>387</v>
       </c>
@@ -5654,7 +5654,7 @@
       </c>
       <c r="E141" s="1"/>
     </row>
-    <row r="142" spans="1:5" ht="192">
+    <row r="142" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>389</v>
       </c>
@@ -5669,7 +5669,7 @@
       </c>
       <c r="E142" s="1"/>
     </row>
-    <row r="143" spans="1:5" ht="207.95">
+    <row r="143" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A143" s="1" t="s">
         <v>392</v>
       </c>
@@ -5684,7 +5684,7 @@
       </c>
       <c r="E143" s="1"/>
     </row>
-    <row r="144" spans="1:5" ht="207.95">
+    <row r="144" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A144" s="1" t="s">
         <v>395</v>
       </c>
@@ -5699,7 +5699,7 @@
       </c>
       <c r="E144" s="1"/>
     </row>
-    <row r="145" spans="1:5" ht="224.1">
+    <row r="145" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A145" s="1" t="s">
         <v>397</v>
       </c>
@@ -5714,7 +5714,7 @@
       </c>
       <c r="E145" s="1"/>
     </row>
-    <row r="146" spans="1:5" ht="224.1">
+    <row r="146" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A146" s="1" t="s">
         <v>400</v>
       </c>
@@ -5729,7 +5729,7 @@
       </c>
       <c r="E146" s="1"/>
     </row>
-    <row r="147" spans="1:5" ht="240">
+    <row r="147" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A147" s="1" t="s">
         <v>403</v>
       </c>
@@ -5744,7 +5744,7 @@
       </c>
       <c r="E147" s="1"/>
     </row>
-    <row r="148" spans="1:5" ht="224.1">
+    <row r="148" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A148" s="1" t="s">
         <v>405</v>
       </c>
@@ -5759,7 +5759,7 @@
       </c>
       <c r="E148" s="1"/>
     </row>
-    <row r="149" spans="1:5" ht="240">
+    <row r="149" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A149" s="1" t="s">
         <v>408</v>
       </c>
@@ -5774,7 +5774,7 @@
       </c>
       <c r="E149" s="1"/>
     </row>
-    <row r="150" spans="1:5" ht="192">
+    <row r="150" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A150" s="1" t="s">
         <v>339</v>
       </c>
@@ -5789,7 +5789,7 @@
       </c>
       <c r="E150" s="1"/>
     </row>
-    <row r="151" spans="1:5" ht="192">
+    <row r="151" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A151" s="1" t="s">
         <v>413</v>
       </c>
@@ -5804,7 +5804,7 @@
       </c>
       <c r="E151" s="1"/>
     </row>
-    <row r="152" spans="1:5" ht="159.94999999999999">
+    <row r="152" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A152" s="1" t="s">
         <v>416</v>
       </c>
@@ -5819,7 +5819,7 @@
       </c>
       <c r="E152" s="1"/>
     </row>
-    <row r="153" spans="1:5" ht="192">
+    <row r="153" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A153" s="1" t="s">
         <v>419</v>
       </c>
@@ -5834,7 +5834,7 @@
       </c>
       <c r="E153" s="1"/>
     </row>
-    <row r="154" spans="1:5" ht="192">
+    <row r="154" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>421</v>
       </c>
@@ -5849,7 +5849,7 @@
       </c>
       <c r="E154" s="1"/>
     </row>
-    <row r="155" spans="1:5" ht="207.95">
+    <row r="155" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A155" s="1" t="s">
         <v>424</v>
       </c>
@@ -5864,7 +5864,7 @@
       </c>
       <c r="E155" s="1"/>
     </row>
-    <row r="156" spans="1:5" ht="192">
+    <row r="156" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A156" s="1" t="s">
         <v>426</v>
       </c>
@@ -5879,7 +5879,7 @@
       </c>
       <c r="E156" s="1"/>
     </row>
-    <row r="157" spans="1:5" ht="240">
+    <row r="157" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A157" s="1" t="s">
         <v>429</v>
       </c>
@@ -5894,7 +5894,7 @@
       </c>
       <c r="E157" s="1"/>
     </row>
-    <row r="158" spans="1:5" ht="224.1">
+    <row r="158" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A158" s="1" t="s">
         <v>432</v>
       </c>
@@ -5909,7 +5909,7 @@
       </c>
       <c r="E158" s="1"/>
     </row>
-    <row r="159" spans="1:5" ht="224.1">
+    <row r="159" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A159" s="1" t="s">
         <v>434</v>
       </c>
@@ -5924,7 +5924,7 @@
       </c>
       <c r="E159" s="1"/>
     </row>
-    <row r="160" spans="1:5" ht="192">
+    <row r="160" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A160" s="1" t="s">
         <v>436</v>
       </c>
@@ -5939,7 +5939,7 @@
       </c>
       <c r="E160" s="1"/>
     </row>
-    <row r="161" spans="1:5" ht="192">
+    <row r="161" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A161" s="1" t="s">
         <v>439</v>
       </c>
@@ -5954,7 +5954,7 @@
       </c>
       <c r="E161" s="1"/>
     </row>
-    <row r="162" spans="1:5" ht="192">
+    <row r="162" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>442</v>
       </c>
@@ -5969,7 +5969,7 @@
       </c>
       <c r="E162" s="1"/>
     </row>
-    <row r="163" spans="1:5" ht="192">
+    <row r="163" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A163" s="1" t="s">
         <v>446</v>
       </c>
@@ -5984,7 +5984,7 @@
       </c>
       <c r="E163" s="1"/>
     </row>
-    <row r="164" spans="1:5" ht="159.94999999999999">
+    <row r="164" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A164" s="1" t="s">
         <v>448</v>
       </c>
@@ -5999,7 +5999,7 @@
       </c>
       <c r="E164" s="1"/>
     </row>
-    <row r="165" spans="1:5" ht="176.1">
+    <row r="165" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A165" s="1" t="s">
         <v>451</v>
       </c>
@@ -6014,7 +6014,7 @@
       </c>
       <c r="E165" s="1"/>
     </row>
-    <row r="166" spans="1:5" ht="176.1">
+    <row r="166" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A166" s="1" t="s">
         <v>454</v>
       </c>
@@ -6029,7 +6029,7 @@
       </c>
       <c r="E166" s="1"/>
     </row>
-    <row r="167" spans="1:5" ht="240">
+    <row r="167" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A167" s="1" t="s">
         <v>456</v>
       </c>
@@ -6044,7 +6044,7 @@
       </c>
       <c r="E167" s="1"/>
     </row>
-    <row r="168" spans="1:5" ht="207.95">
+    <row r="168" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A168" s="1" t="s">
         <v>459</v>
       </c>
@@ -6059,7 +6059,7 @@
       </c>
       <c r="E168" s="1"/>
     </row>
-    <row r="169" spans="1:5" ht="207.95">
+    <row r="169" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A169" s="1" t="s">
         <v>462</v>
       </c>
@@ -6074,7 +6074,7 @@
       </c>
       <c r="E169" s="1"/>
     </row>
-    <row r="170" spans="1:5" ht="176.1">
+    <row r="170" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A170" s="1" t="s">
         <v>465</v>
       </c>
@@ -6089,7 +6089,7 @@
       </c>
       <c r="E170" s="1"/>
     </row>
-    <row r="171" spans="1:5" ht="207.95">
+    <row r="171" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>468</v>
       </c>
@@ -6104,7 +6104,7 @@
       </c>
       <c r="E171" s="1"/>
     </row>
-    <row r="172" spans="1:5" ht="192">
+    <row r="172" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A172" s="1" t="s">
         <v>470</v>
       </c>
@@ -6119,7 +6119,7 @@
       </c>
       <c r="E172" s="1"/>
     </row>
-    <row r="173" spans="1:5" ht="207.95">
+    <row r="173" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A173" s="1" t="s">
         <v>473</v>
       </c>
@@ -6134,7 +6134,7 @@
       </c>
       <c r="E173" s="1"/>
     </row>
-    <row r="174" spans="1:5" ht="192">
+    <row r="174" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A174" s="1" t="s">
         <v>475</v>
       </c>
@@ -6149,7 +6149,7 @@
       </c>
       <c r="E174" s="1"/>
     </row>
-    <row r="175" spans="1:5" ht="192">
+    <row r="175" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A175" s="1" t="s">
         <v>478</v>
       </c>
@@ -6164,7 +6164,7 @@
       </c>
       <c r="E175" s="1"/>
     </row>
-    <row r="176" spans="1:5" ht="240">
+    <row r="176" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A176" s="1" t="s">
         <v>481</v>
       </c>
@@ -6179,7 +6179,7 @@
       </c>
       <c r="E176" s="1"/>
     </row>
-    <row r="177" spans="1:5" ht="176.1">
+    <row r="177" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A177" s="1" t="s">
         <v>484</v>
       </c>
@@ -6194,7 +6194,7 @@
       </c>
       <c r="E177" s="1"/>
     </row>
-    <row r="178" spans="1:5" ht="224.1">
+    <row r="178" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
         <v>486</v>
       </c>
@@ -6209,7 +6209,7 @@
       </c>
       <c r="E178" s="1"/>
     </row>
-    <row r="179" spans="1:5" ht="207.95">
+    <row r="179" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A179" s="1" t="s">
         <v>488</v>
       </c>
@@ -6224,7 +6224,7 @@
       </c>
       <c r="E179" s="1"/>
     </row>
-    <row r="180" spans="1:5" ht="176.1">
+    <row r="180" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A180" s="1" t="s">
         <v>490</v>
       </c>
@@ -6239,7 +6239,7 @@
       </c>
       <c r="E180" s="1"/>
     </row>
-    <row r="181" spans="1:5" ht="192">
+    <row r="181" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A181" s="1" t="s">
         <v>492</v>
       </c>
@@ -6254,7 +6254,7 @@
       </c>
       <c r="E181" s="1"/>
     </row>
-    <row r="182" spans="1:5" ht="255.95">
+    <row r="182" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A182" s="1" t="s">
         <v>495</v>
       </c>
@@ -6269,7 +6269,7 @@
       </c>
       <c r="E182" s="1"/>
     </row>
-    <row r="183" spans="1:5" ht="255.95">
+    <row r="183" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A183" s="1" t="s">
         <v>498</v>
       </c>
@@ -6284,7 +6284,7 @@
       </c>
       <c r="E183" s="1"/>
     </row>
-    <row r="184" spans="1:5" ht="207.95">
+    <row r="184" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A184" s="1" t="s">
         <v>501</v>
       </c>
@@ -6299,7 +6299,7 @@
       </c>
       <c r="E184" s="1"/>
     </row>
-    <row r="185" spans="1:5" ht="192">
+    <row r="185" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A185" s="1" t="s">
         <v>503</v>
       </c>
@@ -6314,7 +6314,7 @@
       </c>
       <c r="E185" s="1"/>
     </row>
-    <row r="186" spans="1:5" ht="240">
+    <row r="186" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A186" s="1" t="s">
         <v>506</v>
       </c>
@@ -6329,7 +6329,7 @@
       </c>
       <c r="E186" s="1"/>
     </row>
-    <row r="187" spans="1:5" ht="207.95">
+    <row r="187" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A187" s="1" t="s">
         <v>509</v>
       </c>
@@ -6344,7 +6344,7 @@
       </c>
       <c r="E187" s="1"/>
     </row>
-    <row r="188" spans="1:5" ht="207.95">
+    <row r="188" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A188" s="1" t="s">
         <v>511</v>
       </c>
@@ -6359,7 +6359,7 @@
       </c>
       <c r="E188" s="1"/>
     </row>
-    <row r="189" spans="1:5" ht="207.95">
+    <row r="189" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A189" s="1" t="s">
         <v>513</v>
       </c>
@@ -6374,7 +6374,7 @@
       </c>
       <c r="E189" s="1"/>
     </row>
-    <row r="190" spans="1:5" ht="207.95">
+    <row r="190" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A190" s="1" t="s">
         <v>516</v>
       </c>
@@ -6389,7 +6389,7 @@
       </c>
       <c r="E190" s="1"/>
     </row>
-    <row r="191" spans="1:5" ht="224.1">
+    <row r="191" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A191" s="1" t="s">
         <v>519</v>
       </c>
@@ -6404,7 +6404,7 @@
       </c>
       <c r="E191" s="1"/>
     </row>
-    <row r="192" spans="1:5" ht="240">
+    <row r="192" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A192" s="1" t="s">
         <v>521</v>
       </c>
@@ -6419,7 +6419,7 @@
       </c>
       <c r="E192" s="1"/>
     </row>
-    <row r="193" spans="1:5" ht="224.1">
+    <row r="193" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A193" s="1" t="s">
         <v>523</v>
       </c>
@@ -6434,7 +6434,7 @@
       </c>
       <c r="E193" s="1"/>
     </row>
-    <row r="194" spans="1:5" ht="176.1">
+    <row r="194" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A194" s="1" t="s">
         <v>526</v>
       </c>
@@ -6449,7 +6449,7 @@
       </c>
       <c r="E194" s="1"/>
     </row>
-    <row r="195" spans="1:5" ht="224.1">
+    <row r="195" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A195" s="1" t="s">
         <v>529</v>
       </c>
@@ -6464,7 +6464,7 @@
       </c>
       <c r="E195" s="1"/>
     </row>
-    <row r="196" spans="1:5" ht="240">
+    <row r="196" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A196" s="1" t="s">
         <v>531</v>
       </c>
@@ -6479,7 +6479,7 @@
       </c>
       <c r="E196" s="1"/>
     </row>
-    <row r="197" spans="1:5" ht="207.95">
+    <row r="197" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A197" s="1" t="s">
         <v>533</v>
       </c>
@@ -6494,7 +6494,7 @@
       </c>
       <c r="E197" s="1"/>
     </row>
-    <row r="198" spans="1:5" ht="240">
+    <row r="198" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A198" s="1" t="s">
         <v>536</v>
       </c>
@@ -6509,7 +6509,7 @@
       </c>
       <c r="E198" s="1"/>
     </row>
-    <row r="199" spans="1:5" ht="192">
+    <row r="199" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A199" s="1" t="s">
         <v>539</v>
       </c>
@@ -6524,7 +6524,7 @@
       </c>
       <c r="E199" s="1"/>
     </row>
-    <row r="200" spans="1:5" ht="224.1">
+    <row r="200" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A200" s="1" t="s">
         <v>542</v>
       </c>
@@ -6539,7 +6539,7 @@
       </c>
       <c r="E200" s="1"/>
     </row>
-    <row r="201" spans="1:5" ht="244.5">
+    <row r="201" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A201" s="1" t="s">
         <v>544</v>
       </c>
@@ -6569,17 +6569,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f482623e-59a6-4eaa-9720-cc6467ba2c24" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4141613b-8dd2-47b8-a22d-41433857583f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F04918ED668FC3429D1FE1FD8AC77EA3" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c20ea19c3d94088dfa2eb857852ee2d2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4141613b-8dd2-47b8-a22d-41433857583f" xmlns:ns3="f482623e-59a6-4eaa-9720-cc6467ba2c24" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="43c99062588a8f0bfb450d784d30b781" ns2:_="" ns3:_="">
     <xsd:import namespace="4141613b-8dd2-47b8-a22d-41433857583f"/>
@@ -6786,14 +6775,51 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f482623e-59a6-4eaa-9720-cc6467ba2c24" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4141613b-8dd2-47b8-a22d-41433857583f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAB712F3-9C88-421A-B93C-32C66C28552C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAB712F3-9C88-421A-B93C-32C66C28552C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5A89D96-988A-41AB-8186-8D1E8C35C8B9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3F4D4F5-1A1D-4785-9DFF-8FE6387EB331}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4141613b-8dd2-47b8-a22d-41433857583f"/>
+    <ds:schemaRef ds:uri="f482623e-59a6-4eaa-9720-cc6467ba2c24"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F3F4D4F5-1A1D-4785-9DFF-8FE6387EB331}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5A89D96-988A-41AB-8186-8D1E8C35C8B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f482623e-59a6-4eaa-9720-cc6467ba2c24"/>
+    <ds:schemaRef ds:uri="4141613b-8dd2-47b8-a22d-41433857583f"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>